<commit_message>
Updated ATB, clean up
-Incorporated new ATB data
-Cleaned up various parts of code
</commit_message>
<xml_diff>
--- a/Python/Data/NewPlantData/NewTechFramework.xlsx
+++ b/Python/Data/NewPlantData/NewTechFramework.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atpha\Documents\Postdocs\Projects\NETs\Model\Python\Data\NewPlantData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtcraig\Desktop\Research\Models\MacroCEM\Python\Data\NewPlantData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92A521C-0CA7-410C-99D7-50292C24FE17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A07009F-A41F-41E0-8062-5E205E72B208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6390" yWindow="360" windowWidth="19335" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NewTechFramework" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="61">
   <si>
     <t>PlantType</t>
   </si>
@@ -91,12 +104,6 @@
     <t>ECAPEX(2012$/MWH)</t>
   </si>
   <si>
-    <t>Coal Steam</t>
-  </si>
-  <si>
-    <t>Coal-new-AvgCF-Mid</t>
-  </si>
-  <si>
     <t>Coal</t>
   </si>
   <si>
@@ -197,9 +204,6 @@
   </si>
   <si>
     <t>CT</t>
-  </si>
-  <si>
-    <t>CS</t>
   </si>
   <si>
     <t>PlantCategory</t>
@@ -1024,10 +1028,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X11"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,39 +1133,39 @@
         <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
       </c>
       <c r="F2">
         <v>650</v>
       </c>
       <c r="K2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L2">
         <v>6.2E-2</v>
       </c>
       <c r="M2">
-        <v>0.11</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="N2">
-        <v>205</v>
+        <v>20.5</v>
       </c>
       <c r="O2">
         <v>65</v>
@@ -1170,63 +1174,63 @@
         <v>0</v>
       </c>
       <c r="Q2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="R2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="S2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="T2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3">
+        <v>400</v>
+      </c>
+      <c r="K3" t="s">
         <v>31</v>
       </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3">
-        <v>650</v>
-      </c>
-      <c r="K3" t="s">
-        <v>33</v>
-      </c>
       <c r="L3">
-        <v>6.2E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="M3">
-        <v>8.5000000000000006E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="N3">
-        <v>20.5</v>
+        <v>119</v>
       </c>
       <c r="O3">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -1235,48 +1239,48 @@
         <v>28</v>
       </c>
       <c r="R3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="T3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
-      </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F4">
-        <v>400</v>
+        <v>340</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L4">
         <v>3.0000000000000001E-3</v>
@@ -1285,7 +1289,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="N4">
-        <v>119</v>
+        <v>11.9</v>
       </c>
       <c r="O4">
         <v>55</v>
@@ -1294,28 +1298,28 @@
         <v>0</v>
       </c>
       <c r="Q4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="S4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="T4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -1323,58 +1327,58 @@
         <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F5">
-        <v>340</v>
+        <v>210</v>
       </c>
       <c r="K5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="L5">
-        <v>3.0000000000000001E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="M5">
-        <v>3.5000000000000003E-2</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="N5">
-        <v>11.9</v>
+        <v>119</v>
       </c>
       <c r="O5">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="P5">
         <v>0</v>
       </c>
       <c r="Q5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="S5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="T5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X5" t="s">
         <v>56</v>
@@ -1385,84 +1389,87 @@
         <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
         <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F6">
-        <v>210</v>
+        <v>1117</v>
       </c>
       <c r="K6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L6">
-        <v>8.9999999999999993E-3</v>
+        <v>0</v>
       </c>
       <c r="M6">
-        <v>8.6999999999999994E-2</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>119</v>
+        <v>0</v>
       </c>
       <c r="O6">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="P6">
         <v>0</v>
       </c>
       <c r="Q6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="S6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="T6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X6" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
         <v>42</v>
       </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="F7">
-        <v>1117</v>
+        <v>500</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -1474,60 +1481,60 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="P7">
         <v>0</v>
       </c>
       <c r="Q7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="S7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="T7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X7" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
         <v>44</v>
       </c>
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" t="s">
-        <v>46</v>
-      </c>
       <c r="F8">
-        <v>500</v>
+        <v>100</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1539,51 +1546,51 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="P8">
         <v>0</v>
       </c>
       <c r="Q8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="S8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="T8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="V8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="W8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="X8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F9">
         <v>100</v>
@@ -1592,7 +1599,7 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1604,60 +1611,62 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="P9">
         <v>0</v>
       </c>
       <c r="Q9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R9" t="s">
-        <v>30</v>
-      </c>
-      <c r="S9" t="s">
-        <v>30</v>
-      </c>
-      <c r="T9" t="s">
-        <v>30</v>
-      </c>
-      <c r="U9" t="s">
-        <v>30</v>
-      </c>
-      <c r="V9" t="s">
-        <v>30</v>
-      </c>
-      <c r="W9" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="S9">
+        <v>0.81</v>
+      </c>
+      <c r="T9">
+        <f>F9*4</f>
+        <v>400</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <f>F9</f>
+        <v>100</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
       </c>
       <c r="X9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
         <v>50</v>
       </c>
-      <c r="B10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>51</v>
       </c>
-      <c r="D10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" t="s">
-        <v>53</v>
-      </c>
       <c r="F10">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1675,94 +1684,27 @@
         <v>0</v>
       </c>
       <c r="Q10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="S10">
         <v>0.81</v>
       </c>
       <c r="T10">
-        <f>F10*4</f>
-        <v>400</v>
+        <f>F10*4*30*24</f>
+        <v>1440000</v>
       </c>
       <c r="U10">
         <v>0</v>
       </c>
       <c r="V10">
         <f>F10</f>
-        <v>100</v>
-      </c>
-      <c r="W10">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="X10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
         <v>52</v>
-      </c>
-      <c r="E11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11">
-        <v>500</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="K11" t="s">
-        <v>33</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>15</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>30</v>
-      </c>
-      <c r="R11" t="s">
-        <v>30</v>
-      </c>
-      <c r="S11">
-        <v>0.81</v>
-      </c>
-      <c r="T11">
-        <f>F11*4*30*24</f>
-        <v>1440000</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-      <c r="V11">
-        <f>F11</f>
-        <v>500</v>
-      </c>
-      <c r="X11" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>